<commit_message>
cambios a la tabla
</commit_message>
<xml_diff>
--- a/Tabla.xlsx
+++ b/Tabla.xlsx
@@ -32,7 +32,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -55,13 +55,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,104 +380,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:E10"/>
+  <dimension ref="C2:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C2" s="1">
         <v>3</v>
       </c>
       <c r="D2" s="1">
         <v>12</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1">
+        <v>222</v>
+      </c>
+      <c r="G2" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C3" s="1">
         <v>3</v>
       </c>
       <c r="D3" s="1">
         <v>22</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1">
+        <v>222</v>
+      </c>
+      <c r="G3" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C4" s="1">
         <v>3</v>
       </c>
       <c r="D4" s="1">
         <v>22</v>
       </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="2">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>222</v>
+      </c>
+      <c r="G4" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C5" s="1">
         <v>3</v>
       </c>
       <c r="D5" s="1">
         <v>22</v>
       </c>
-      <c r="E5" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="2">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>222</v>
+      </c>
+      <c r="G5" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C6" s="1">
         <v>3</v>
       </c>
       <c r="D6" s="1">
         <v>22</v>
       </c>
-      <c r="E6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+      <c r="F6" s="1">
+        <v>222</v>
+      </c>
+      <c r="G6" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C7" s="1">
         <v>3</v>
       </c>
       <c r="D7" s="1">
         <v>22</v>
       </c>
-      <c r="E7" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="2">
+        <v>3</v>
+      </c>
+      <c r="F7" s="1">
+        <v>222</v>
+      </c>
+      <c r="G7" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C8" s="1">
         <v>3</v>
       </c>
       <c r="D8" s="1">
         <v>22</v>
       </c>
-      <c r="E8" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="2">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1">
+        <v>222</v>
+      </c>
+      <c r="G8" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>3</v>
       </c>
       <c r="D9" s="1">
         <v>22</v>
       </c>
-      <c r="E9" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
+      <c r="F9" s="1">
+        <v>222</v>
+      </c>
+      <c r="G9" s="1">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
+      <c r="F10" s="1">
+        <v>222</v>
+      </c>
+      <c r="G10" s="1">
+        <v>225</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>